<commit_message>
Schottky-Diode packages filled in.
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@20313 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Schottky-Diodes.xlsx
+++ b/Digikey/Schottky-Diodes.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Stephen Deiss\Gadgetron\Gadgets\Libraries\Parts\Digikey\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="609" activeTab="2"/>
+    <workbookView xWindow="555" yWindow="555" windowWidth="25035" windowHeight="15495" tabRatio="609" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="5" r:id="rId1"/>
     <sheet name="SOD-323" sheetId="1" r:id="rId2"/>
     <sheet name="TH" sheetId="17" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="244">
   <si>
     <t>ï»¿"Datasheets"</t>
   </si>
@@ -158,9 +163,6 @@
     <t>Micro Commercial Co</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 200MA SOD323</t>
-  </si>
-  <si>
     <t>Schottky</t>
   </si>
   <si>
@@ -191,18 +193,12 @@
     <t>125Â°C (Max)</t>
   </si>
   <si>
-    <t>http://www.mccsemi.com/up_pdf/BAT42WS-BAT43WS(SOD323).pdf</t>
-  </si>
-  <si>
     <t>BAT43WSTPMSCT-ND</t>
   </si>
   <si>
     <t>BAT43WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 100MA SOD323</t>
-  </si>
-  <si>
     <t>100mA</t>
   </si>
   <si>
@@ -227,9 +223,6 @@
     <t>RB751V-40-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 30MA SOD323</t>
-  </si>
-  <si>
     <t>30mA</t>
   </si>
   <si>
@@ -248,9 +241,6 @@
     <t>RB500V-40-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 100MA SOD323</t>
-  </si>
-  <si>
     <t>40V</t>
   </si>
   <si>
@@ -272,9 +262,6 @@
     <t>B5817WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 20V 1A SOD323</t>
-  </si>
-  <si>
     <t>1A</t>
   </si>
   <si>
@@ -299,9 +286,6 @@
     <t>RB551V-30-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 20V 500MA SOD323</t>
-  </si>
-  <si>
     <t>500mA</t>
   </si>
   <si>
@@ -332,27 +316,18 @@
     <t>B5818WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 1A SOD323</t>
-  </si>
-  <si>
     <t>550mV @ 1A</t>
   </si>
   <si>
     <t>1mA @ 30V</t>
   </si>
   <si>
-    <t>http://www.mccsemi.com/up_pdf/B0530WS(SOD323).pdf</t>
-  </si>
-  <si>
     <t>B0530WS-TPMSCT-ND</t>
   </si>
   <si>
     <t>B0530WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 500MA SOD323</t>
-  </si>
-  <si>
     <t>550mV @ 500mA</t>
   </si>
   <si>
@@ -365,9 +340,6 @@
     <t>B5819WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 1A SOD323</t>
-  </si>
-  <si>
     <t>600mV @ 1A</t>
   </si>
   <si>
@@ -383,9 +355,6 @@
     <t>SD103AWS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 350MA SOD323</t>
-  </si>
-  <si>
     <t>350mA</t>
   </si>
   <si>
@@ -404,9 +373,6 @@
     <t>SD103BWS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 350MA SOD323</t>
-  </si>
-  <si>
     <t>5ÂµA @ 20V</t>
   </si>
   <si>
@@ -416,9 +382,6 @@
     <t>SD103CWS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 20V 350MA SOD323</t>
-  </si>
-  <si>
     <t>5ÂµA @ 10V</t>
   </si>
   <si>
@@ -431,9 +394,6 @@
     <t>BSR106WS-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 60V 1A SOD323</t>
-  </si>
-  <si>
     <t>60V</t>
   </si>
   <si>
@@ -461,18 +421,12 @@
     <t>-55Â°C ~ 150Â°C</t>
   </si>
   <si>
-    <t>http://media.digikey.com/pdf/Data%20Sheets/Micro%20Commercial%20PDFs/MBRX02520-MBRX02560(SOD323).pdf</t>
-  </si>
-  <si>
     <t>MBRX02520TPMSCT-ND</t>
   </si>
   <si>
     <t>MBRX02520-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 20V 250MA SOD323</t>
-  </si>
-  <si>
     <t>250mA</t>
   </si>
   <si>
@@ -488,9 +442,6 @@
     <t>MBRX02530-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 250MA SOD323</t>
-  </si>
-  <si>
     <t>550mV @ 250mA</t>
   </si>
   <si>
@@ -503,9 +454,6 @@
     <t>MBRX02540-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 250MA SOD323</t>
-  </si>
-  <si>
     <t>500ÂµA @ 40V</t>
   </si>
   <si>
@@ -515,9 +463,6 @@
     <t>MBRX02550-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 50V 250MA SOD323</t>
-  </si>
-  <si>
     <t>700mV @ 250mA</t>
   </si>
   <si>
@@ -530,15 +475,9 @@
     <t>MBRX02560-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 60V 250MA SOD323</t>
-  </si>
-  <si>
     <t>500ÂµA @ 60V</t>
   </si>
   <si>
-    <t>http://media.digikey.com/pdf/Data%20Sheets/Micro%20Commercial%20PDFs/MBRX0520-MBRX0560(SOD323).pdf</t>
-  </si>
-  <si>
     <t>MBRX0520TPMSCT-ND</t>
   </si>
   <si>
@@ -563,9 +502,6 @@
     <t>MBRX0540-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 500MA SOD323</t>
-  </si>
-  <si>
     <t>300ÂµA @ 40V</t>
   </si>
   <si>
@@ -575,9 +511,6 @@
     <t>MBRX0560-TP</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 60V 500MA SOD323</t>
-  </si>
-  <si>
     <t>700mV @ 500mA</t>
   </si>
   <si>
@@ -740,7 +673,91 @@
     <t>Device</t>
   </si>
   <si>
-    <t>SOD323</t>
+    <t>SOD2512X100_HS</t>
+  </si>
+  <si>
+    <t>SOD3716X135_HS</t>
+  </si>
+  <si>
+    <t>DIOAD1125W78L520D270_HS</t>
+  </si>
+  <si>
+    <t>DIOAD2120W125L950D530_HS</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 200MA SOD-323</t>
+  </si>
+  <si>
+    <t>http://www.mccsemi.com/up_pdf/BAT42WS-BAT43WS(SOD-323).pdf</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 100MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 30MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 100MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 1A SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 500MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 1A SOD-323</t>
+  </si>
+  <si>
+    <t>http://www.mccsemi.com/up_pdf/B0530WS(SOD-323).pdf</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 500MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 350MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 350MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 350MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 60V 1A SOD-323</t>
+  </si>
+  <si>
+    <t>http://media.digikey.com/pdf/Data%20Sheets/Micro%20Commercial%20PDFs/MBRX02520-MBRX02560(SOD-323).pdf</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 250MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 250MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 250MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 50V 250MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 60V 250MA SOD-323</t>
+  </si>
+  <si>
+    <t>http://media.digikey.com/pdf/Data%20Sheets/Micro%20Commercial%20PDFs/MBRX0520-MBRX0560(SOD-323).pdf</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 500MA SOD-323</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 60V 500MA SOD-323</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
   </si>
 </sst>
 </file>
@@ -940,11 +957,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1069,6 +1089,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1482,36 +1510,36 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
   </sheetData>
@@ -1529,40 +1557,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <pane xSplit="30300" topLeftCell="AC1"/>
-      <selection activeCell="AB27" sqref="AB27"/>
-      <selection pane="topRight" activeCell="AD388" sqref="AD388"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane xSplit="30300" topLeftCell="Y1" activePane="topRight"/>
+      <selection activeCell="X7" sqref="X7"/>
+      <selection pane="topRight" activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="14.625" customWidth="1"/>
+    <col min="9" max="9" width="16.875" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="12" max="12" width="11.875" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
+    <col min="15" max="15" width="29.375" customWidth="1"/>
     <col min="16" max="16" width="29" customWidth="1"/>
-    <col min="17" max="17" width="30.6640625" customWidth="1"/>
-    <col min="18" max="18" width="50.33203125" customWidth="1"/>
-    <col min="19" max="19" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="30.625" customWidth="1"/>
+    <col min="18" max="18" width="50.375" customWidth="1"/>
+    <col min="19" max="19" width="26.375" customWidth="1"/>
     <col min="20" max="20" width="29.5" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="16.1640625" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="16.125" customWidth="1"/>
+    <col min="23" max="23" width="15.875" customWidth="1"/>
     <col min="24" max="24" width="23.5" customWidth="1"/>
-    <col min="25" max="25" width="31.33203125" customWidth="1"/>
-    <col min="26" max="30" width="11" customWidth="1"/>
+    <col min="25" max="25" width="31.375" customWidth="1"/>
+    <col min="26" max="26" width="10.875" customWidth="1"/>
+    <col min="27" max="27" width="18.125" customWidth="1"/>
+    <col min="28" max="30" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16" thickBot="1">
+    <row r="1" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1675,7 @@
         <v>22</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="AC1" t="s">
         <v>25</v>
@@ -1654,7 +1684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16" thickTop="1">
+    <row r="2" spans="1:30" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1671,7 +1701,7 @@
         <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="G2">
         <v>50688</v>
@@ -1695,25 +1725,25 @@
         <v>18</v>
       </c>
       <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>47</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>49</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>50</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>51</v>
-      </c>
-      <c r="T2" t="s">
-        <v>52</v>
       </c>
       <c r="U2" t="s">
         <v>18</v>
@@ -1722,36 +1752,42 @@
         <v>27</v>
       </c>
       <c r="W2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" t="s">
         <v>54</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>55</v>
       </c>
       <c r="Z2" t="s">
         <v>23</v>
       </c>
+      <c r="AA2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="G3">
         <v>9495</v>
@@ -1775,25 +1811,25 @@
         <v>18</v>
       </c>
       <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
         <v>46</v>
       </c>
-      <c r="O3" t="s">
-        <v>47</v>
-      </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" t="s">
         <v>50</v>
       </c>
-      <c r="S3" t="s">
-        <v>51</v>
-      </c>
       <c r="T3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U3" t="s">
         <v>18</v>
@@ -1802,10 +1838,10 @@
         <v>27</v>
       </c>
       <c r="W3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y3" t="s">
         <v>17</v>
@@ -1813,25 +1849,31 @@
       <c r="Z3" t="s">
         <v>23</v>
       </c>
+      <c r="AA3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="G4">
         <v>9084</v>
@@ -1855,25 +1897,25 @@
         <v>18</v>
       </c>
       <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
         <v>46</v>
       </c>
-      <c r="O4" t="s">
-        <v>47</v>
-      </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R4" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" t="s">
         <v>50</v>
       </c>
-      <c r="S4" t="s">
-        <v>51</v>
-      </c>
       <c r="T4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s">
         <v>18</v>
@@ -1882,10 +1924,10 @@
         <v>27</v>
       </c>
       <c r="W4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y4" t="s">
         <v>17</v>
@@ -1893,25 +1935,31 @@
       <c r="Z4" t="s">
         <v>23</v>
       </c>
+      <c r="AA4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="G5">
         <v>7238</v>
@@ -1935,63 +1983,69 @@
         <v>18</v>
       </c>
       <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
         <v>46</v>
       </c>
-      <c r="O5" t="s">
-        <v>47</v>
-      </c>
       <c r="P5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S5" t="s">
         <v>18</v>
       </c>
       <c r="T5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="V5" t="s">
         <v>27</v>
       </c>
       <c r="W5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y5" t="s">
         <v>54</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>55</v>
       </c>
       <c r="Z5" t="s">
         <v>23</v>
       </c>
+      <c r="AA5" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="G6">
         <v>9527</v>
@@ -2015,63 +2069,69 @@
         <v>18</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S6" t="s">
         <v>18</v>
       </c>
       <c r="T6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="U6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="V6" t="s">
         <v>27</v>
       </c>
       <c r="W6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y6" t="s">
         <v>54</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>55</v>
       </c>
       <c r="Z6" t="s">
         <v>23</v>
       </c>
+      <c r="AA6" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>224</v>
       </c>
       <c r="G7">
         <v>22636</v>
@@ -2095,25 +2155,25 @@
         <v>18</v>
       </c>
       <c r="N7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O7" t="s">
         <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="R7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S7" t="s">
         <v>18</v>
       </c>
       <c r="T7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="U7" t="s">
         <v>18</v>
@@ -2122,36 +2182,42 @@
         <v>27</v>
       </c>
       <c r="W7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z7" t="s">
         <v>23</v>
       </c>
+      <c r="AA7" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="G8">
         <v>15634</v>
@@ -2175,25 +2241,25 @@
         <v>18</v>
       </c>
       <c r="N8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O8" t="s">
         <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="R8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S8" t="s">
         <v>18</v>
       </c>
       <c r="T8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="U8" t="s">
         <v>18</v>
@@ -2202,36 +2268,42 @@
         <v>27</v>
       </c>
       <c r="W8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y8" t="s">
         <v>54</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>55</v>
       </c>
       <c r="Z8" t="s">
         <v>23</v>
       </c>
+      <c r="AA8" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="G9">
         <v>13747</v>
@@ -2255,63 +2327,69 @@
         <v>18</v>
       </c>
       <c r="N9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="R9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S9" t="s">
         <v>18</v>
       </c>
       <c r="T9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="U9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="V9" t="s">
         <v>27</v>
       </c>
       <c r="W9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" t="s">
         <v>54</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>55</v>
       </c>
       <c r="Z9" t="s">
         <v>23</v>
       </c>
+      <c r="AA9" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="G10">
         <v>369</v>
@@ -2335,25 +2413,25 @@
         <v>18</v>
       </c>
       <c r="N10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" t="s">
         <v>46</v>
       </c>
-      <c r="O10" t="s">
-        <v>47</v>
-      </c>
       <c r="P10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="R10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S10" t="s">
         <v>18</v>
       </c>
       <c r="T10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="U10" t="s">
         <v>18</v>
@@ -2362,36 +2440,42 @@
         <v>27</v>
       </c>
       <c r="W10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z10" t="s">
         <v>23</v>
       </c>
+      <c r="AA10" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>228</v>
       </c>
       <c r="G11">
         <v>1534</v>
@@ -2415,25 +2499,25 @@
         <v>18</v>
       </c>
       <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" t="s">
         <v>46</v>
       </c>
-      <c r="O11" t="s">
-        <v>47</v>
-      </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S11" t="s">
         <v>18</v>
       </c>
       <c r="T11" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="U11" t="s">
         <v>18</v>
@@ -2442,10 +2526,10 @@
         <v>27</v>
       </c>
       <c r="W11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y11" t="s">
         <v>17</v>
@@ -2453,25 +2537,31 @@
       <c r="Z11" t="s">
         <v>23</v>
       </c>
+      <c r="AA11" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="G12">
         <v>87700</v>
@@ -2495,25 +2585,25 @@
         <v>18</v>
       </c>
       <c r="N12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q12" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S12" t="s">
         <v>18</v>
       </c>
       <c r="T12" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="U12" t="s">
         <v>18</v>
@@ -2522,36 +2612,42 @@
         <v>27</v>
       </c>
       <c r="W12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z12" t="s">
         <v>23</v>
       </c>
+      <c r="AA12" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E13" t="s">
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="G13">
         <v>27557</v>
@@ -2575,25 +2671,25 @@
         <v>18</v>
       </c>
       <c r="N13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="Q13" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="R13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S13" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="T13" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="U13" t="s">
         <v>18</v>
@@ -2602,36 +2698,42 @@
         <v>27</v>
       </c>
       <c r="W13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z13" t="s">
         <v>23</v>
       </c>
+      <c r="AA13" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>231</v>
       </c>
       <c r="G14">
         <v>20633</v>
@@ -2655,25 +2757,25 @@
         <v>18</v>
       </c>
       <c r="N14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14" t="s">
         <v>46</v>
       </c>
-      <c r="O14" t="s">
-        <v>47</v>
-      </c>
       <c r="P14" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="Q14" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="R14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S14" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="T14" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="U14" t="s">
         <v>18</v>
@@ -2682,36 +2784,42 @@
         <v>27</v>
       </c>
       <c r="W14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z14" t="s">
         <v>23</v>
       </c>
+      <c r="AA14" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2735,25 +2843,25 @@
         <v>18</v>
       </c>
       <c r="N15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O15" t="s">
         <v>19</v>
       </c>
       <c r="P15" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="Q15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="R15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S15" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="T15" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="U15" t="s">
         <v>18</v>
@@ -2762,36 +2870,42 @@
         <v>27</v>
       </c>
       <c r="W15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z15" t="s">
         <v>23</v>
       </c>
+      <c r="AA15" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>136</v>
+        <v>233</v>
       </c>
       <c r="G16">
         <v>2532</v>
@@ -2815,25 +2929,25 @@
         <v>18</v>
       </c>
       <c r="N16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="P16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q16" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="R16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S16" t="s">
         <v>18</v>
       </c>
       <c r="T16" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="U16" t="s">
         <v>18</v>
@@ -2842,36 +2956,42 @@
         <v>27</v>
       </c>
       <c r="W16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Z16" t="s">
         <v>23</v>
       </c>
+      <c r="AA16" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="G17">
         <v>47530</v>
@@ -2895,25 +3015,25 @@
         <v>18</v>
       </c>
       <c r="N17" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" t="s">
         <v>46</v>
       </c>
-      <c r="O17" t="s">
-        <v>47</v>
-      </c>
       <c r="P17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q17" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="R17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S17" t="s">
         <v>18</v>
       </c>
       <c r="T17" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="U17" t="s">
         <v>18</v>
@@ -2922,36 +3042,42 @@
         <v>27</v>
       </c>
       <c r="W17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y17" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="Z17" t="s">
         <v>23</v>
       </c>
+      <c r="AA17" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
+        <v>235</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2975,25 +3101,25 @@
         <v>18</v>
       </c>
       <c r="N18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" t="s">
         <v>19</v>
       </c>
       <c r="P18" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="Q18" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="R18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S18" t="s">
         <v>18</v>
       </c>
       <c r="T18" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="U18" t="s">
         <v>18</v>
@@ -3002,33 +3128,39 @@
         <v>27</v>
       </c>
       <c r="W18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y18" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="AA18" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>155</v>
+        <v>236</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -3052,25 +3184,25 @@
         <v>18</v>
       </c>
       <c r="N19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" t="s">
         <v>46</v>
       </c>
-      <c r="O19" t="s">
-        <v>47</v>
-      </c>
       <c r="P19" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="Q19" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="R19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S19" t="s">
         <v>18</v>
       </c>
       <c r="T19" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="U19" t="s">
         <v>18</v>
@@ -3079,33 +3211,39 @@
         <v>27</v>
       </c>
       <c r="W19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y19" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E20" t="s">
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>160</v>
+        <v>237</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3129,25 +3267,25 @@
         <v>18</v>
       </c>
       <c r="N20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P20" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="Q20" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="R20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S20" t="s">
         <v>18</v>
       </c>
       <c r="T20" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="U20" t="s">
         <v>18</v>
@@ -3156,33 +3294,39 @@
         <v>27</v>
       </c>
       <c r="W20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y20" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -3206,25 +3350,25 @@
         <v>18</v>
       </c>
       <c r="N21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O21" t="s">
         <v>16</v>
       </c>
       <c r="P21" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="Q21" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="R21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S21" t="s">
         <v>18</v>
       </c>
       <c r="T21" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="U21" t="s">
         <v>18</v>
@@ -3233,33 +3377,39 @@
         <v>27</v>
       </c>
       <c r="W21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y21" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="AA21" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>239</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -3283,25 +3433,25 @@
         <v>18</v>
       </c>
       <c r="N22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O22" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="P22" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="Q22" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="R22" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S22" t="s">
         <v>18</v>
       </c>
       <c r="T22" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="U22" t="s">
         <v>18</v>
@@ -3310,33 +3460,39 @@
         <v>27</v>
       </c>
       <c r="W22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y22" t="s">
-        <v>145</v>
+        <v>130</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -3360,25 +3516,25 @@
         <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O23" t="s">
         <v>19</v>
       </c>
       <c r="P23" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q23" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="R23" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S23" t="s">
         <v>18</v>
       </c>
       <c r="T23" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="U23" t="s">
         <v>18</v>
@@ -3387,33 +3543,39 @@
         <v>27</v>
       </c>
       <c r="W23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y23" t="s">
         <v>17</v>
       </c>
+      <c r="AA23" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>228</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -3437,25 +3599,25 @@
         <v>18</v>
       </c>
       <c r="N24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" t="s">
         <v>46</v>
       </c>
-      <c r="O24" t="s">
-        <v>47</v>
-      </c>
       <c r="P24" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q24" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S24" t="s">
         <v>18</v>
       </c>
       <c r="T24" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="U24" t="s">
         <v>18</v>
@@ -3464,33 +3626,39 @@
         <v>27</v>
       </c>
       <c r="W24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y24" t="s">
         <v>17</v>
       </c>
+      <c r="AA24" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>180</v>
+        <v>241</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -3514,25 +3682,25 @@
         <v>18</v>
       </c>
       <c r="N25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q25" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="R25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S25" t="s">
         <v>18</v>
       </c>
       <c r="T25" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="U25" t="s">
         <v>18</v>
@@ -3541,33 +3709,39 @@
         <v>27</v>
       </c>
       <c r="W25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y25" t="s">
         <v>17</v>
       </c>
+      <c r="AA25" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="E26" t="s">
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>184</v>
+        <v>242</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -3591,25 +3765,25 @@
         <v>18</v>
       </c>
       <c r="N26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O26" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="P26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="Q26" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="R26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S26" t="s">
         <v>18</v>
       </c>
       <c r="T26" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="U26" t="s">
         <v>18</v>
@@ -3618,33 +3792,39 @@
         <v>27</v>
       </c>
       <c r="W26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y26" t="s">
         <v>17</v>
       </c>
+      <c r="AA26" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="G27" s="1">
         <v>46290</v>
@@ -3668,25 +3848,25 @@
         <v>18</v>
       </c>
       <c r="N27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="P27" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>18</v>
@@ -3695,20 +3875,22 @@
         <v>27</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA27" s="1"/>
+      <c r="AA27" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="AB27" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
@@ -3716,9 +3898,9 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3732,36 +3914,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <pane xSplit="14340" topLeftCell="W1"/>
-      <selection activeCell="AB7" sqref="AB7"/>
-      <selection pane="topRight" activeCell="AB1" sqref="AB1"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <pane xSplit="14340" topLeftCell="V1" activePane="topRight"/>
+      <selection activeCell="AA4" sqref="AA4"/>
+      <selection pane="topRight" activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="10" width="4.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="4.625" customWidth="1"/>
+    <col min="9" max="10" width="4.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="13" width="3.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="3.875" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.875" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="17.375" customWidth="1"/>
+    <col min="27" max="27" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="16" thickBot="1">
+    <row r="1" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3844,27 +4027,27 @@
         <v>22</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="16" thickTop="1">
+    <row r="2" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="G2">
         <v>25698</v>
@@ -3888,25 +4071,25 @@
         <v>18</v>
       </c>
       <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
-        <v>47</v>
-      </c>
       <c r="P2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q2" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s">
         <v>18</v>
       </c>
       <c r="T2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="U2" t="s">
         <v>18</v>
@@ -3915,33 +4098,39 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="X2" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="Y2" t="s">
-        <v>207</v>
+        <v>183</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="G3">
         <v>10410</v>
@@ -3965,25 +4154,25 @@
         <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s">
         <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="R3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S3" t="s">
         <v>18</v>
       </c>
       <c r="T3" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="U3" t="s">
         <v>18</v>
@@ -3992,39 +4181,42 @@
         <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="X3" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="Y3" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="Z3" t="s">
         <v>24</v>
       </c>
+      <c r="AA3" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="AB3" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="G4">
         <v>3784</v>
@@ -4048,25 +4240,25 @@
         <v>18</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P4" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="Q4" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="R4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S4" t="s">
         <v>18</v>
       </c>
       <c r="T4" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="U4" t="s">
         <v>18</v>
@@ -4075,39 +4267,42 @@
         <v>26</v>
       </c>
       <c r="W4" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="X4" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="Y4" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="Z4" t="s">
         <v>24</v>
       </c>
+      <c r="AA4" s="4" t="s">
+        <v>218</v>
+      </c>
       <c r="AB4" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F5" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="G5">
         <v>229</v>
@@ -4131,25 +4326,25 @@
         <v>18</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="P5" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="Q5" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="R5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S5" t="s">
         <v>18</v>
       </c>
       <c r="T5" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="U5" t="s">
         <v>18</v>
@@ -4158,33 +4353,39 @@
         <v>26</v>
       </c>
       <c r="W5" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="X5" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="Y5" t="s">
-        <v>207</v>
+        <v>183</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" t="s">
         <v>202</v>
-      </c>
-      <c r="F6" t="s">
-        <v>226</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4208,25 +4409,25 @@
         <v>18</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O6" t="s">
         <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="Q6" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="R6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S6" t="s">
         <v>18</v>
       </c>
       <c r="T6" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="U6" t="s">
         <v>18</v>
@@ -4235,33 +4436,39 @@
         <v>26</v>
       </c>
       <c r="W6" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="X6" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="Y6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="7" spans="1:28">
-      <c r="A7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" t="s">
-        <v>231</v>
-      </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F7" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4285,25 +4492,25 @@
         <v>18</v>
       </c>
       <c r="N7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
         <v>46</v>
       </c>
-      <c r="O7" t="s">
-        <v>47</v>
-      </c>
       <c r="P7" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="Q7" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="R7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S7" t="s">
         <v>18</v>
       </c>
       <c r="T7" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="U7" t="s">
         <v>18</v>
@@ -4312,21 +4519,27 @@
         <v>26</v>
       </c>
       <c r="W7" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="X7" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="Y7" t="s">
-        <v>207</v>
+        <v>183</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>